<commit_message>
Instantiate board from property data
</commit_message>
<xml_diff>
--- a/Software_Engineering/BoardData/PropertyTycoonBoardData.xlsx
+++ b/Software_Engineering/BoardData/PropertyTycoonBoardData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24220" windowHeight="8380"/>
+    <workbookView xWindow="2740" yWindow="0" windowWidth="24220" windowHeight="12140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="89">
   <si>
     <t>Go</t>
   </si>
@@ -187,9 +187,6 @@
   </si>
   <si>
     <t>Go to Jail</t>
-  </si>
-  <si>
-    <t>Go to jail</t>
   </si>
   <si>
     <t>Sirat Mews</t>
@@ -298,7 +295,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -322,6 +319,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -340,15 +353,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -663,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -673,6 +694,7 @@
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="14.83203125" customWidth="1"/>
     <col min="6" max="6" width="10.5" customWidth="1"/>
+    <col min="7" max="7" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20">
@@ -698,7 +720,7 @@
         <v>5</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>7</v>
@@ -724,7 +746,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>12</v>
@@ -733,25 +755,25 @@
         <v>3</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -883,7 +905,7 @@
         <v>200</v>
       </c>
       <c r="G10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1068,7 +1090,7 @@
         <v>150</v>
       </c>
       <c r="G17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1158,7 +1180,7 @@
         <v>200</v>
       </c>
       <c r="G20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1166,7 +1188,7 @@
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C21" t="s">
         <v>39</v>
@@ -1430,7 +1452,7 @@
         <v>200</v>
       </c>
       <c r="G30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -1520,7 +1542,7 @@
         <v>150</v>
       </c>
       <c r="G33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -1565,9 +1587,6 @@
       <c r="B35" t="s">
         <v>54</v>
       </c>
-      <c r="C35" t="s">
-        <v>55</v>
-      </c>
       <c r="E35" t="s">
         <v>14</v>
       </c>
@@ -1577,10 +1596,10 @@
         <v>32</v>
       </c>
       <c r="B36" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" t="s">
         <v>56</v>
-      </c>
-      <c r="C36" t="s">
-        <v>57</v>
       </c>
       <c r="E36" t="s">
         <v>18</v>
@@ -1612,10 +1631,10 @@
         <v>33</v>
       </c>
       <c r="B37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E37" t="s">
         <v>18</v>
@@ -1661,10 +1680,10 @@
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E39" t="s">
         <v>18</v>
@@ -1696,7 +1715,7 @@
         <v>36</v>
       </c>
       <c r="B40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C40" t="s">
         <v>25</v>
@@ -1708,7 +1727,7 @@
         <v>200</v>
       </c>
       <c r="G40" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -1718,7 +1737,7 @@
       <c r="B41" t="s">
         <v>28</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>20</v>
       </c>
       <c r="E41" t="s">
@@ -1730,10 +1749,10 @@
         <v>38</v>
       </c>
       <c r="B42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E42" t="s">
         <v>18</v>
@@ -1765,10 +1784,10 @@
         <v>39</v>
       </c>
       <c r="B43" t="s">
+        <v>61</v>
+      </c>
+      <c r="D43" t="s">
         <v>62</v>
-      </c>
-      <c r="D43" t="s">
-        <v>63</v>
       </c>
       <c r="E43" t="s">
         <v>14</v>
@@ -1779,10 +1798,10 @@
         <v>40</v>
       </c>
       <c r="B44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E44" t="s">
         <v>18</v>
@@ -1811,75 +1830,75 @@
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47" spans="1:12">
       <c r="A47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H47" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="48" spans="1:12">
       <c r="A48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F48" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H48" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F49" t="s">
+        <v>81</v>
+      </c>
+      <c r="H49" t="s">
         <v>82</v>
-      </c>
-      <c r="H49" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F50" t="s">
+        <v>83</v>
+      </c>
+      <c r="H50" t="s">
         <v>84</v>
-      </c>
-      <c r="H50" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F51" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H51" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="52" spans="1:12">
       <c r="A52" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:12">
       <c r="A53" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:12" s="1" customFormat="1">

</xml_diff>